<commit_message>
End formula corrected. Some advancements on the doc.
</commit_message>
<xml_diff>
--- a/Semestre_i_DFMEA_Temperance.xlsx
+++ b/Semestre_i_DFMEA_Temperance.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
   <si>
     <t>Process or Product Name:</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Requerimiento 7</t>
   </si>
   <si>
-    <t>El commando llego trunco</t>
-  </si>
-  <si>
     <t>El commando llego modificado</t>
   </si>
   <si>
@@ -373,15 +370,6 @@
     <t>Occurrence (customer)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sin conexion </t>
-  </si>
-  <si>
-    <t>Falso en el cableado</t>
-  </si>
-  <si>
-    <t>Cadena Portacables</t>
-  </si>
-  <si>
     <t>SPARC (TEMPERANCE)</t>
   </si>
   <si>
@@ -422,6 +410,42 @@
   </si>
   <si>
     <t>Tener que reiniciar el sistema o reconectarlo.</t>
+  </si>
+  <si>
+    <t>Sin conexión.</t>
+  </si>
+  <si>
+    <t>No está energizado.</t>
+  </si>
+  <si>
+    <t>Hay un cortocircuito.</t>
+  </si>
+  <si>
+    <t>Usar indicadores LED de encendido.</t>
+  </si>
+  <si>
+    <t>Jorge Sáenz</t>
+  </si>
+  <si>
+    <t>El commando llego trunco.</t>
+  </si>
+  <si>
+    <t>Sólo hace una parte de la instrucción.</t>
+  </si>
+  <si>
+    <t>Falso en el cableado.</t>
+  </si>
+  <si>
+    <t>Mal baudaje.</t>
+  </si>
+  <si>
+    <t>El string sde envió incompleto.</t>
+  </si>
+  <si>
+    <t>Cadena portacables.</t>
+  </si>
+  <si>
+    <t>SPARC avisa si el string estuvo incompleto.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +510,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +553,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -935,7 +965,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1078,9 +1108,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1089,9 +1116,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1163,22 +1187,220 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1187,213 +1409,46 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="28" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1403,7 +1458,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1457,7 +1532,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B23317E6-8623-41F0-8B0D-8D4182394236}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B23317E6-8623-41F0-8B0D-8D4182394236}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1564,7 +1639,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E63FA1D0-9A8D-4AE7-AA03-2C872B4E63FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E63FA1D0-9A8D-4AE7-AA03-2C872B4E63FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1613,7 +1688,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A218B3AF-48DA-48E5-9731-2C4A17B13FE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A218B3AF-48DA-48E5-9731-2C4A17B13FE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1720,7 +1795,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D06A2989-DB73-4D40-81D8-2706C13BEA5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D06A2989-DB73-4D40-81D8-2706C13BEA5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1846,7 @@
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B1952D4-D5C3-44C8-B55C-7329C3042AA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B1952D4-D5C3-44C8-B55C-7329C3042AA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1868,7 +1943,7 @@
         <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA69449B-4546-4D4C-B035-C63AC3E43DFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA69449B-4546-4D4C-B035-C63AC3E43DFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1919,7 +1994,7 @@
         <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9807E8F4-898B-4ACB-BEC9-A3A3CE12A11A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9807E8F4-898B-4ACB-BEC9-A3A3CE12A11A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2016,7 +2091,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A81C25D7-CE9C-4064-A6FA-1A0F35148A44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A81C25D7-CE9C-4064-A6FA-1A0F35148A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2067,7 +2142,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD792D50-326C-4B7B-BC13-74A3B2411AC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD792D50-326C-4B7B-BC13-74A3B2411AC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2239,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE6999E-2B84-4E83-8AF6-CF17F4F1AE95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DE6999E-2B84-4E83-8AF6-CF17F4F1AE95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2215,7 +2290,7 @@
         <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC65B1C1-FF46-41B2-B49B-47BA29375766}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC65B1C1-FF46-41B2-B49B-47BA29375766}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2312,7 +2387,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{895F1EB6-18C0-4E56-8307-A2ABB2EEE9F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{895F1EB6-18C0-4E56-8307-A2ABB2EEE9F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2363,7 +2438,7 @@
         <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{130776FA-1B6D-48C1-92E2-7300C66F5515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{130776FA-1B6D-48C1-92E2-7300C66F5515}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2460,7 +2535,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29E24126-67C1-4809-9342-BF4654D11587}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29E24126-67C1-4809-9342-BF4654D11587}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2511,7 +2586,7 @@
         <xdr:cNvPr id="16" name="TextBox 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814BF6D2-2D92-4757-A2E1-53B67E3D2A2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{814BF6D2-2D92-4757-A2E1-53B67E3D2A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2614,7 +2689,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A97B86A-BBC3-4E71-AE61-6B58F40E52CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A97B86A-BBC3-4E71-AE61-6B58F40E52CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2665,7 +2740,7 @@
         <xdr:cNvPr id="18" name="TextBox 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7571F63-536C-4E5A-B3AE-107982A09057}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A7571F63-536C-4E5A-B3AE-107982A09057}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2768,7 +2843,7 @@
         <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E121374-3D38-4DD3-B80B-8541354BAC32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E121374-3D38-4DD3-B80B-8541354BAC32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2819,7 +2894,7 @@
         <xdr:cNvPr id="20" name="TextBox 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACEE8AC5-BD67-43DD-A54B-0E22E06FF988}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACEE8AC5-BD67-43DD-A54B-0E22E06FF988}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2922,7 +2997,7 @@
         <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3FE31C-2044-41A1-9CBF-F9799A6B59B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EF3FE31C-2044-41A1-9CBF-F9799A6B59B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2973,7 +3048,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE725C70-7C8B-48CF-AD74-39829B1635E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CE725C70-7C8B-48CF-AD74-39829B1635E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3067,7 +3142,7 @@
         <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD56E8A-D17A-4A1D-BC90-EC22B99F70A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BD56E8A-D17A-4A1D-BC90-EC22B99F70A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3118,7 +3193,7 @@
         <xdr:cNvPr id="24" name="Left Brace 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D5DA83-2044-475D-8918-F2D8D7DFFA66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1D5DA83-2044-475D-8918-F2D8D7DFFA66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3175,7 +3250,7 @@
         <xdr:cNvPr id="25" name="TextBox 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{613FE002-EC1B-48D1-AF14-5A5EAED7513B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{613FE002-EC1B-48D1-AF14-5A5EAED7513B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3310,7 +3385,7 @@
         <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629B6D83-BDE4-42F7-93D7-559AD3CC9BF2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{629B6D83-BDE4-42F7-93D7-559AD3CC9BF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3649,8 +3724,8 @@
   </sheetPr>
   <dimension ref="A1:W447"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3670,7 +3745,8 @@
     <col min="14" max="14" width="85.28515625" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="16" width="5.85546875" customWidth="1"/>
-    <col min="17" max="18" width="3.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" customWidth="1"/>
     <col min="21" max="21" width="51.140625" customWidth="1"/>
     <col min="22" max="22" width="32.7109375" customWidth="1"/>
@@ -3681,21 +3757,21 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="93"/>
+      <c r="B1" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="96"/>
+      <c r="H1" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="2"/>
@@ -3707,19 +3783,19 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="94"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="102"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="2"/>
@@ -3843,7 +3919,7 @@
       <c r="M5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="114" t="s">
+      <c r="N5" s="73" t="s">
         <v>34</v>
       </c>
       <c r="O5" s="19"/>
@@ -3852,732 +3928,855 @@
       <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="83"/>
-      <c r="B6" s="72" t="s">
+      <c r="A6" s="98"/>
+      <c r="B6" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="103" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="106" t="s">
+      <c r="C6" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="68">
+        <v>8</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="68">
+        <v>5</v>
+      </c>
+      <c r="H6" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="108">
+      <c r="I6" s="55">
         <v>8</v>
       </c>
-      <c r="F6" s="116" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="108">
-        <v>5</v>
-      </c>
-      <c r="H6" s="107" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" s="57">
-        <v>8</v>
-      </c>
       <c r="J6" s="23">
-        <f>$E$6*$G$6*I6</f>
+        <f>E6*G6*I6</f>
         <v>320</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="108">
+      <c r="N6" s="74"/>
+      <c r="O6" s="68">
         <f>E6</f>
         <v>8</v>
       </c>
-      <c r="P6" s="108">
+      <c r="P6" s="68">
         <f>$G$6</f>
         <v>5</v>
       </c>
-      <c r="Q6" s="107"/>
+      <c r="Q6" s="67">
+        <v>4</v>
+      </c>
       <c r="R6" s="26">
-        <f>O$6*P6*Q6</f>
-        <v>0</v>
+        <f>O6*P6*Q6</f>
+        <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="108">
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="99"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="68">
         <v>5</v>
       </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="27"/>
+      <c r="F7" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="68">
+        <v>10</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="27">
+        <v>1</v>
+      </c>
       <c r="J7" s="23">
-        <f t="shared" ref="J7:J8" si="0">$E$6*$G$6*I7</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="22"/>
+        <f t="shared" ref="J7:J44" si="0">E7*G7*I7</f>
+        <v>50</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>109</v>
+      </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="115"/>
-      <c r="O7" s="108">
+      <c r="N7" s="74"/>
+      <c r="O7" s="68">
         <v>5</v>
       </c>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="107"/>
+      <c r="P7" s="68">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="67">
+        <v>1</v>
+      </c>
       <c r="R7" s="26">
-        <f>O$6*P6*Q7</f>
-        <v>0</v>
+        <f t="shared" ref="R7:R44" si="1">O7*P7*Q7</f>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="106" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" s="108">
+      <c r="A8" s="99"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="68">
         <v>5</v>
       </c>
-      <c r="F8" s="117"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="27"/>
+      <c r="F8" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="68">
+        <v>10</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1</v>
+      </c>
       <c r="J8" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>99</v>
+      </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="115"/>
-      <c r="O8" s="108">
+      <c r="N8" s="74"/>
+      <c r="O8" s="68">
         <v>5</v>
       </c>
-      <c r="P8" s="108"/>
-      <c r="Q8" s="107"/>
+      <c r="P8" s="68">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="67">
+        <v>1</v>
+      </c>
       <c r="R8" s="26">
-        <f>O$6*P6*Q8</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="27"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="127"/>
       <c r="J9" s="23">
-        <f>$E$6*$G$6*I9</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="115"/>
-      <c r="O9" s="113"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="107"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="128"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="131"/>
+      <c r="O9" s="132"/>
+      <c r="P9" s="124"/>
+      <c r="Q9" s="126"/>
       <c r="R9" s="26">
-        <f>O$6*P6*Q9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="84"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="103" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="108">
+      <c r="A10" s="99"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="68">
         <v>5</v>
       </c>
-      <c r="F10" s="117" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="108">
+      <c r="F10" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="68">
         <v>3</v>
       </c>
-      <c r="H10" s="107"/>
-      <c r="I10" s="27"/>
+      <c r="H10" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="27">
+        <v>7</v>
+      </c>
       <c r="J10" s="23">
-        <f>$E$10*$G$6*I10</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>105</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="L10" s="22"/>
+        <v>115</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>109</v>
+      </c>
       <c r="M10" s="28"/>
-      <c r="N10" s="115"/>
-      <c r="O10" s="108">
+      <c r="N10" s="74"/>
+      <c r="O10" s="68">
         <f>E10</f>
         <v>5</v>
       </c>
-      <c r="P10" s="108">
-        <f>$G$10</f>
-        <v>3</v>
-      </c>
-      <c r="Q10" s="107"/>
+      <c r="P10" s="68">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>6</v>
+      </c>
       <c r="R10" s="26">
-        <f>O$10*P$10*Q10</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="58"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="68">
+        <v>8</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="68">
+        <v>4</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="56">
+        <v>8</v>
+      </c>
       <c r="J11" s="23">
-        <f>$E$10*$G$10*I11</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="22"/>
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>99</v>
+      </c>
       <c r="M11" s="28"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="113"/>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="107"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="68">
+        <f t="shared" ref="O11:O13" si="2">E11</f>
+        <v>8</v>
+      </c>
+      <c r="P11" s="68">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="67">
+        <v>6</v>
+      </c>
       <c r="R11" s="26">
-        <f>O$10*P$10*Q11</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="27"/>
+    <row r="12" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="79">
+        <v>7</v>
+      </c>
+      <c r="F12" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="68">
+        <v>7</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="27">
+        <v>1</v>
+      </c>
       <c r="J12" s="23">
-        <f>$E$10*$G$10*I12</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="22"/>
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>99</v>
+      </c>
       <c r="M12" s="28"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="113"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="107"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="68">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="P12" s="68">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="67">
+        <v>1</v>
+      </c>
       <c r="R12" s="26">
-        <f>O$10*P$10*Q12</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="103" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="106" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="108">
+      <c r="A13" s="99"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="68">
         <v>5</v>
       </c>
-      <c r="F13" s="66" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="78">
+      <c r="F13" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="68">
         <v>2</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="27"/>
       <c r="J13" s="23">
-        <f>$E$13*$G$13*I13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13" s="24"/>
       <c r="L13" s="22"/>
       <c r="M13" s="28"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="110">
-        <f>E13</f>
+      <c r="N13" s="77"/>
+      <c r="O13" s="68">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P13" s="78">
-        <f t="shared" ref="P13:P21" si="1">G13</f>
+      <c r="P13" s="70">
+        <f t="shared" ref="P13:P21" si="3">G13</f>
         <v>2</v>
       </c>
       <c r="Q13" s="27"/>
       <c r="R13" s="26">
-        <f>O$13*P$13*Q13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="107" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="79"/>
-      <c r="H14" s="22"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="68"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="27"/>
       <c r="J14" s="23">
-        <f>$E$13*$G$13*I14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14" s="24"/>
       <c r="L14" s="22"/>
       <c r="M14" s="28"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="79"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="71"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="26">
-        <f>O$13*P$13*Q14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="121" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="124">
+      <c r="A15" s="99"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="83">
         <v>6</v>
       </c>
-      <c r="F15" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="68">
+      <c r="F15" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="65">
         <v>1</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="23"/>
+      <c r="J15" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K15" s="24"/>
       <c r="L15" s="22"/>
       <c r="M15" s="28"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
       <c r="Q15" s="27"/>
-      <c r="R15" s="26"/>
+      <c r="R15" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="125" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="123"/>
-      <c r="H16" s="107"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="82"/>
+      <c r="H16" s="67"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="23"/>
+      <c r="J16" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K16" s="24"/>
       <c r="L16" s="22"/>
       <c r="M16" s="28"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
       <c r="Q16" s="27"/>
-      <c r="R16" s="26"/>
+      <c r="R16" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="84"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="122" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="123"/>
-      <c r="F17" s="117" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="123"/>
-      <c r="H17" s="107"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="81" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="82"/>
+      <c r="F17" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="82"/>
+      <c r="H17" s="67"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="23"/>
+      <c r="J17" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K17" s="24"/>
       <c r="L17" s="22"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
       <c r="Q17" s="27"/>
-      <c r="R17" s="26"/>
+      <c r="R17" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="84"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="117" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="123"/>
-      <c r="H18" s="107"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="82"/>
+      <c r="H18" s="67"/>
       <c r="I18" s="27"/>
-      <c r="J18" s="23"/>
+      <c r="J18" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K18" s="24"/>
       <c r="L18" s="22"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="63"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
       <c r="Q18" s="27"/>
-      <c r="R18" s="26"/>
+      <c r="R18" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="123"/>
-      <c r="F19" s="117" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="123"/>
-      <c r="H19" s="107"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="82"/>
+      <c r="F19" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="82"/>
+      <c r="H19" s="67"/>
       <c r="I19" s="27"/>
-      <c r="J19" s="23"/>
+      <c r="J19" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K19" s="24"/>
       <c r="L19" s="22"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
       <c r="Q19" s="27"/>
-      <c r="R19" s="26"/>
+      <c r="R19" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="107"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="67"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="23"/>
+      <c r="J20" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K20" s="24"/>
       <c r="L20" s="22"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
       <c r="Q20" s="27"/>
-      <c r="R20" s="26"/>
+      <c r="R20" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="103" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="106" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="108"/>
-      <c r="F21" s="117" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="108"/>
-      <c r="H21" s="107"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="68"/>
+      <c r="H21" s="67"/>
       <c r="I21" s="27"/>
       <c r="J21" s="23">
-        <f>$E$21*$G$21*I21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K21" s="24"/>
       <c r="L21" s="22"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="109">
+      <c r="N21" s="107"/>
+      <c r="O21" s="69">
         <f>E21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="109">
-        <f t="shared" si="1"/>
+      <c r="P21" s="69">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q21" s="27"/>
       <c r="R21" s="26">
-        <f>O$21*P$21*Q21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="107"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="67"/>
       <c r="I22" s="27"/>
       <c r="J22" s="23">
-        <f t="shared" ref="J22" si="2">$E$21*$G$21*I22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="22"/>
       <c r="M22" s="28"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="126"/>
-      <c r="P22" s="110"/>
+      <c r="N22" s="108"/>
+      <c r="O22" s="85"/>
+      <c r="P22" s="70"/>
       <c r="Q22" s="27"/>
       <c r="R22" s="26">
-        <f t="shared" ref="R22" si="3">O$21*P$21*Q22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="84"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="107"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="67"/>
       <c r="I23" s="27"/>
       <c r="J23" s="23">
-        <f>$E$21*$G$21*I23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="22"/>
       <c r="M23" s="28"/>
-      <c r="N23" s="90"/>
-      <c r="O23" s="112"/>
-      <c r="P23" s="111"/>
+      <c r="N23" s="109"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="71"/>
       <c r="Q23" s="27"/>
       <c r="R23" s="26">
-        <f>O$21*P$21*Q23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="78"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="78"/>
+      <c r="G24" s="105"/>
       <c r="H24" s="22"/>
       <c r="I24" s="27"/>
       <c r="J24" s="23">
-        <f>$E$24*$G$24*I24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K24" s="29"/>
       <c r="L24" s="29"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="109">
+      <c r="N24" s="116"/>
+      <c r="O24" s="69">
         <f>E24</f>
         <v>0</v>
       </c>
-      <c r="P24" s="109">
+      <c r="P24" s="69">
         <f t="shared" ref="P24:P43" si="4">G24</f>
         <v>0</v>
       </c>
       <c r="Q24" s="22"/>
       <c r="R24" s="26">
-        <f>O$24*P24*Q24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="84"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="78"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="105"/>
       <c r="H25" s="22"/>
       <c r="I25" s="27"/>
       <c r="J25" s="23">
-        <f t="shared" ref="J25:J27" si="5">$E$24*$G$24*I25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K25" s="29"/>
       <c r="L25" s="29"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="110"/>
-      <c r="P25" s="110"/>
+      <c r="N25" s="118"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="70"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="26">
-        <f t="shared" ref="R25:R29" si="6">O$24*P25*Q25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="84"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="78"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="105"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="78"/>
+      <c r="G26" s="105"/>
       <c r="H26" s="22"/>
       <c r="I26" s="27"/>
       <c r="J26" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
       <c r="M26" s="28"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="110"/>
-      <c r="P26" s="110"/>
+      <c r="N26" s="118"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="79"/>
+      <c r="A27" s="99"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="106"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="79"/>
+      <c r="G27" s="106"/>
       <c r="H27" s="22"/>
       <c r="I27" s="27"/>
       <c r="J27" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
       <c r="M27" s="28"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="110"/>
-      <c r="P27" s="111"/>
+      <c r="N27" s="117"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="71"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="78"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="105"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="86"/>
+      <c r="G28" s="114"/>
       <c r="H28" s="22"/>
       <c r="I28" s="27"/>
       <c r="J28" s="23">
-        <f>$E$28*$G$28*I28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
       <c r="M28" s="28"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="109">
+      <c r="N28" s="116"/>
+      <c r="O28" s="69">
         <f>E28</f>
         <v>0</v>
       </c>
-      <c r="P28" s="109">
+      <c r="P28" s="69">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q28" s="22"/>
       <c r="R28" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="85"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="79"/>
+      <c r="A29" s="110"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="106"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="87"/>
+      <c r="G29" s="115"/>
       <c r="H29" s="22"/>
       <c r="I29" s="27"/>
       <c r="J29" s="23">
-        <f>$E$28*$G$28*I29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K29" s="32"/>
       <c r="L29" s="32"/>
       <c r="M29" s="28"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="111"/>
+      <c r="N29" s="117"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="71"/>
       <c r="Q29" s="22"/>
       <c r="R29" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="69"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="119"/>
       <c r="F30" s="22"/>
-      <c r="G30" s="69"/>
+      <c r="G30" s="119"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="59"/>
+      <c r="I30" s="57"/>
       <c r="J30" s="23">
-        <f>$E$30*$G$30*I30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30" s="24"/>
       <c r="L30" s="22"/>
       <c r="M30" s="28"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="69">
+      <c r="N30" s="116"/>
+      <c r="O30" s="119">
         <f>E35</f>
         <v>0</v>
       </c>
@@ -4587,109 +4786,109 @@
       </c>
       <c r="Q30" s="22"/>
       <c r="R30" s="26">
-        <f>O$30*P30*Q30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="84"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="78"/>
+      <c r="A31" s="99"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="105"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="59"/>
+      <c r="I31" s="57"/>
       <c r="J31" s="23">
-        <f t="shared" ref="J31:J32" si="7">$E$30*$G$30*I31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K31" s="24"/>
       <c r="L31" s="22"/>
       <c r="M31" s="28"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="78"/>
+      <c r="N31" s="118"/>
+      <c r="O31" s="105"/>
       <c r="P31" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q31" s="22"/>
       <c r="R31" s="26">
-        <f>O$30*P31*Q31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="84"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="78"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="105"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="59"/>
+      <c r="I32" s="57"/>
       <c r="J32" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K32" s="24"/>
       <c r="L32" s="22"/>
       <c r="M32" s="28"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="78"/>
+      <c r="N32" s="118"/>
+      <c r="O32" s="105"/>
       <c r="P32" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q32" s="22"/>
       <c r="R32" s="26">
-        <f t="shared" ref="R32:R38" si="8">O$30*P32*Q32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="84"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="79"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="113"/>
+      <c r="D33" s="113"/>
+      <c r="E33" s="106"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="79"/>
+      <c r="G33" s="106"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="59"/>
+      <c r="I33" s="57"/>
       <c r="J33" s="23">
-        <f>$E$30*$G$30*I33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K33" s="24"/>
       <c r="L33" s="22"/>
       <c r="M33" s="28"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="79"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="106"/>
       <c r="P33" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q33" s="22"/>
       <c r="R33" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="84"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
+      <c r="A34" s="99"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="22"/>
       <c r="G34" s="27"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="59"/>
+      <c r="I34" s="57"/>
       <c r="J34" s="23">
-        <f>$E$34*$G$34*I34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K34" s="24"/>
@@ -4706,29 +4905,29 @@
       </c>
       <c r="Q34" s="27"/>
       <c r="R34" s="26">
-        <f>O$30*P34*Q34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="84"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="69"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="119"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="69"/>
+      <c r="G35" s="119"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="59"/>
+      <c r="I35" s="57"/>
       <c r="J35" s="23">
-        <f>$E$35*$G$35*I35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K35" s="24"/>
       <c r="L35" s="22"/>
       <c r="M35" s="28"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="69">
+      <c r="N35" s="116"/>
+      <c r="O35" s="119">
         <f>E35</f>
         <v>0</v>
       </c>
@@ -4738,116 +4937,116 @@
       </c>
       <c r="Q35" s="22"/>
       <c r="R35" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="84"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="78"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="105"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="59"/>
+      <c r="I36" s="57"/>
       <c r="J36" s="23">
-        <f t="shared" ref="J36:J37" si="9">$E$35*$G$35*I36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K36" s="24"/>
       <c r="L36" s="22"/>
       <c r="M36" s="28"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="70"/>
+      <c r="N36" s="118"/>
+      <c r="O36" s="120"/>
       <c r="P36" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q36" s="22"/>
       <c r="R36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="84"/>
-      <c r="B37" s="73"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="78"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="105"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="59"/>
+      <c r="I37" s="57"/>
       <c r="J37" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K37" s="24"/>
       <c r="L37" s="22"/>
       <c r="M37" s="28"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="70"/>
+      <c r="N37" s="118"/>
+      <c r="O37" s="120"/>
       <c r="P37" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q37" s="22"/>
       <c r="R37" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="85"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="79"/>
+      <c r="A38" s="110"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="106"/>
       <c r="F38" s="22"/>
-      <c r="G38" s="79"/>
+      <c r="G38" s="106"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="59"/>
+      <c r="I38" s="57"/>
       <c r="J38" s="23">
-        <f>$E$35*$G$35*I38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K38" s="24"/>
       <c r="L38" s="22"/>
       <c r="M38" s="28"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="71"/>
+      <c r="N38" s="117"/>
+      <c r="O38" s="121"/>
       <c r="P38" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q38" s="22"/>
       <c r="R38" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="69"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="111"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="119"/>
       <c r="F39" s="22"/>
-      <c r="G39" s="69"/>
+      <c r="G39" s="119"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="59"/>
+      <c r="I39" s="57"/>
       <c r="J39" s="23">
-        <f>$E$39*$G$39:$G$43*I39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K39" s="24"/>
       <c r="L39" s="22"/>
       <c r="M39" s="28"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="69">
+      <c r="N39" s="116"/>
+      <c r="O39" s="119">
         <f>E39</f>
         <v>0</v>
       </c>
@@ -4857,123 +5056,123 @@
       </c>
       <c r="Q39" s="22"/>
       <c r="R39" s="26">
-        <f>O$39*P39*Q39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="84"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="78"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="112"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="105"/>
       <c r="H40" s="22"/>
-      <c r="I40" s="59"/>
+      <c r="I40" s="57"/>
       <c r="J40" s="23">
-        <f t="shared" ref="J40:J43" si="10">$E$39*$G$39:$G$43*I40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K40" s="24"/>
       <c r="L40" s="22"/>
       <c r="M40" s="28"/>
-      <c r="N40" s="76"/>
-      <c r="O40" s="70"/>
+      <c r="N40" s="118"/>
+      <c r="O40" s="120"/>
       <c r="P40" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q40" s="22"/>
       <c r="R40" s="26">
-        <f t="shared" ref="R40:R42" si="11">O$39*P40*Q40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="84"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="78"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="105"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="59"/>
+      <c r="I41" s="57"/>
       <c r="J41" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K41" s="24"/>
       <c r="L41" s="22"/>
       <c r="M41" s="28"/>
-      <c r="N41" s="76"/>
-      <c r="O41" s="70"/>
+      <c r="N41" s="118"/>
+      <c r="O41" s="120"/>
       <c r="P41" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q41" s="22"/>
       <c r="R41" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="84"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="78"/>
+      <c r="A42" s="99"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="105"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="59"/>
+      <c r="I42" s="57"/>
       <c r="J42" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K42" s="24"/>
       <c r="L42" s="22"/>
       <c r="M42" s="28"/>
-      <c r="N42" s="76"/>
-      <c r="O42" s="70"/>
+      <c r="N42" s="118"/>
+      <c r="O42" s="120"/>
       <c r="P42" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q42" s="22"/>
       <c r="R42" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
-      <c r="B43" s="74"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="79"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="122"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="113"/>
+      <c r="E43" s="106"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="79"/>
+      <c r="G43" s="106"/>
       <c r="H43" s="22"/>
-      <c r="I43" s="59"/>
+      <c r="I43" s="57"/>
       <c r="J43" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K43" s="24"/>
       <c r="L43" s="22"/>
       <c r="M43" s="28"/>
-      <c r="N43" s="77"/>
-      <c r="O43" s="71"/>
+      <c r="N43" s="117"/>
+      <c r="O43" s="121"/>
       <c r="P43" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q43" s="22"/>
       <c r="R43" s="26">
-        <f>O$39*P43*Q43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4999,7 +5198,10 @@
         <v>40</v>
       </c>
       <c r="I44" s="40"/>
-      <c r="J44" s="42"/>
+      <c r="J44" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K44" s="41" t="s">
         <v>41</v>
       </c>
@@ -5009,27 +5211,30 @@
       <c r="M44" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="N44" s="43" t="s">
+      <c r="N44" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="45"/>
-      <c r="T44" s="46"/>
-      <c r="U44" s="47"/>
-      <c r="V44" s="48"/>
-      <c r="W44" s="48"/>
+      <c r="O44" s="43"/>
+      <c r="P44" s="43"/>
+      <c r="Q44" s="43"/>
+      <c r="R44" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="44"/>
+      <c r="U44" s="45"/>
+      <c r="V44" s="46"/>
+      <c r="W44" s="46"/>
     </row>
     <row r="45" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="48"/>
-      <c r="V45" s="48"/>
-      <c r="W45" s="48"/>
+      <c r="C45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="T45" s="44"/>
+      <c r="U45" s="46"/>
+      <c r="V45" s="46"/>
+      <c r="W45" s="46"/>
     </row>
     <row r="46" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5434,41 +5639,7 @@
     <row r="446" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="447" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="A6:A23"/>
-    <mergeCell ref="B6:B23"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="N21:N23"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="N24:N27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="E39:E43"/>
-    <mergeCell ref="G39:G43"/>
+  <mergeCells count="46">
     <mergeCell ref="O39:O43"/>
     <mergeCell ref="B24:B29"/>
     <mergeCell ref="B30:B33"/>
@@ -5483,8 +5654,40 @@
     <mergeCell ref="N35:N38"/>
     <mergeCell ref="O35:O38"/>
     <mergeCell ref="N30:N33"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="E39:E43"/>
+    <mergeCell ref="G39:G43"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="N24:N27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="N21:N23"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="A6:A23"/>
+    <mergeCell ref="B6:B23"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
-  <conditionalFormatting sqref="J6:J43">
+  <conditionalFormatting sqref="J6:J44">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5495,14 +5698,14 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:R43">
+  <conditionalFormatting sqref="R6:R44">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -5530,8 +5733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5543,154 +5746,154 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="50" t="s">
         <v>90</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53">
+      <c r="A3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="52" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53">
+      <c r="A4" s="51">
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="52" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53">
+      <c r="A5" s="51">
         <v>3</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53">
+      <c r="A6" s="51">
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="52" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
+      <c r="A7" s="51">
         <v>5</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="52" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53">
+      <c r="A8" s="51">
         <v>6</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="52" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53">
+      <c r="A9" s="51">
         <v>7</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="52" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
+      <c r="A10" s="51">
         <v>8</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="52" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="51">
         <v>9</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="52" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
+      <c r="A12" s="51">
         <v>10</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="52" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5701,21 +5904,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008627D652ECF16F40ADBE374E3D3D87F6" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a82faf83e130f03aec18d17d2520a96e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fb007535-a6a4-4ea0-86da-29f43c46b391" xmlns:ns3="b4c971ed-d55e-45d5-823f-e5f0a4d5378a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87a257aab2ea2865cd171ccfb5db57b0" ns2:_="" ns3:_="">
     <xsd:import namespace="fb007535-a6a4-4ea0-86da-29f43c46b391"/>
@@ -5880,24 +6068,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D99D69-C41B-42E2-B319-512FDE30DA9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{321A4371-70D3-4670-B9DE-51C73593625E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE32DFB4-4620-4CB8-8357-3506FC850A95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5914,4 +6100,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{321A4371-70D3-4670-B9DE-51C73593625E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D99D69-C41B-42E2-B319-512FDE30DA9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>